<commit_message>
Instead of getting rid of missaligned cycles, now it realignes them
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/analysis/divers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE944FE-5F69-F941-B8D6-EB6FB58A55F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE13E6F-F3A4-2148-91D0-11E6F9C5E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
   <sheets>
     <sheet name="Tri runs" sheetId="9" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Pn 82Ga" sheetId="16" r:id="rId4"/>
     <sheet name="Eff 84Ga" sheetId="15" r:id="rId5"/>
     <sheet name="Pn 84Ga" sheetId="14" r:id="rId6"/>
-    <sheet name="Calbration RUN58" sheetId="7" r:id="rId7"/>
-    <sheet name="Comparaison reglages beta" sheetId="4" r:id="rId8"/>
-    <sheet name="Calcul Pn 82Ga avec RUN29" sheetId="6" r:id="rId9"/>
-    <sheet name="RUN51" sheetId="10" r:id="rId10"/>
-    <sheet name="RUN55" sheetId="13" r:id="rId11"/>
-    <sheet name="RUN56" sheetId="11" r:id="rId12"/>
-    <sheet name="RUN61" sheetId="12" r:id="rId13"/>
+    <sheet name="P2n 84Ga" sheetId="17" r:id="rId7"/>
+    <sheet name="Calbration RUN58" sheetId="7" r:id="rId8"/>
+    <sheet name="Comparaison reglages beta" sheetId="4" r:id="rId9"/>
+    <sheet name="Calcul Pn 82Ga avec RUN29" sheetId="6" r:id="rId10"/>
+    <sheet name="RUN51" sheetId="10" r:id="rId11"/>
+    <sheet name="RUN55" sheetId="13" r:id="rId12"/>
+    <sheet name="RUN56" sheetId="11" r:id="rId13"/>
+    <sheet name="RUN61" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="206">
   <si>
     <t>Pn</t>
   </si>
@@ -640,13 +641,31 @@
     <t>Les deux valeurs sont bien cohérentes</t>
   </si>
   <si>
-    <t>Ratio beta/neutron</t>
-  </si>
-  <si>
     <t>Courbe activité beta moche</t>
   </si>
   <si>
     <t>20, 29</t>
+  </si>
+  <si>
+    <t>Méthode n-n</t>
+  </si>
+  <si>
+    <t>N2n</t>
+  </si>
+  <si>
+    <t>Reff</t>
+  </si>
+  <si>
+    <t>Effn</t>
+  </si>
+  <si>
+    <t>P2n</t>
+  </si>
+  <si>
+    <t>Nb</t>
+  </si>
+  <si>
+    <t>Ratio eff beta/neutron</t>
   </si>
 </sst>
 </file>
@@ -1861,6 +1880,81 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1B99CB8-DB0E-B400-7A2E-1497CC3126D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7150100" y="368300"/>
+          <a:ext cx="2641600" cy="1397000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Ici j'ai pris le ratio calculé pour Pn 84Ga et j'ai pris Effn qui conserve ce ratio avec l'efficacité beta de 82Ga</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>580571</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -2185,7 +2279,42 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:txDef>
+      <a:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+      <a:lstStyle>
+        <a:defPPr algn="l">
+          <a:defRPr sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:defRPr>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </a:style>
+    </a:txDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -2199,7 +2328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6887EF2-46CF-E446-B33F-5F6D80182EE1}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2460,7 +2589,7 @@
         <v>125</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>124</v>
@@ -2543,6 +2672,194 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BAEB1E-CF2C-6A4E-B6C2-6EA04F34FC3D}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="10.625" style="1"/>
+    <col min="3" max="3" width="8.875" style="1" customWidth="1"/>
+    <col min="4" max="9" width="10.625" style="1"/>
+    <col min="10" max="10" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18">
+      <c r="C1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1467.21</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(SQRT(2*PI())*C6*C4)</f>
+        <v>4175.7542079112691</v>
+      </c>
+      <c r="G4" s="1">
+        <f>E9/E4</f>
+        <v>0.53247653583503463</v>
+      </c>
+      <c r="H4" s="1">
+        <f>E14/E4</f>
+        <v>0.5671611174999649</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1443030</v>
+      </c>
+      <c r="K4" s="7">
+        <v>11382700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18">
+      <c r="C5" s="9">
+        <v>711.02300000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18">
+      <c r="C6" s="9">
+        <v>1.13541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="18">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="6">
+        <v>780.23099999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <f>(SQRT(2*PI())*C11*C9)</f>
+        <v>2223.4911351271617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18">
+      <c r="C10" s="6">
+        <v>709.88199999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18">
+      <c r="C11" s="6">
+        <v>1.1369</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="I12" s="1">
+        <f>(J4/K4)*(H21/G4)*100</f>
+        <v>15.579447179280329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
+        <v>840.09100000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <f>(SQRT(2*PI())*C16*C14)</f>
+        <v>2368.3254229641361</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="18">
+      <c r="C15" s="6">
+        <v>709.85400000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18">
+      <c r="C16" s="6">
+        <v>1.1246700000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18">
+      <c r="C19" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4558.08</v>
+      </c>
+      <c r="E21" s="1">
+        <f>(SQRT(2*PI())*C23*C21)</f>
+        <v>15138.785427111903</v>
+      </c>
+      <c r="H21" s="1">
+        <f>E26/E21</f>
+        <v>0.65436859451512963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18">
+      <c r="C22" s="6">
+        <v>1348.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18">
+      <c r="C23" s="6">
+        <v>1.32501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2999.78</v>
+      </c>
+      <c r="E26" s="1">
+        <f>(SQRT(2*PI())*C28*C26)</f>
+        <v>9906.3457426053428</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18">
+      <c r="C27" s="6">
+        <v>1348.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18">
+      <c r="C28" s="6">
+        <v>1.31745</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7680E834-25BF-554B-A055-DB729B0B172B}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -2726,7 +3043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB024FC4-B85F-3448-8E2A-E4C44EA629AC}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2790,7 +3107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B3A609-792A-7642-9CAD-67077A136A92}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2892,7 +3209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFF8B5B-F9EE-F84C-8391-8E968454A576}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -2964,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6376C050-E39F-4E43-B6D2-85F3F9FA265F}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C25"/>
+    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3656,7 +3973,7 @@
         <v>9.5</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18">
@@ -3690,7 +4007,7 @@
         <v>9</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18">
@@ -4162,7 +4479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFFCE4E-1904-9441-B800-76A5932E8BAB}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="J8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -5411,7 +5728,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5509,7 +5826,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5685,12 +6002,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" style="1" bestFit="1" customWidth="1"/>
@@ -5704,7 +6021,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="5" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>180</v>
@@ -5723,15 +6040,15 @@
       <c r="A2" s="3">
         <v>1.5209999999999999</v>
       </c>
-      <c r="B2" s="6">
-        <v>210092</v>
-      </c>
-      <c r="C2" s="6">
-        <v>902950</v>
+      <c r="B2" s="27">
+        <v>215776</v>
+      </c>
+      <c r="C2" s="27">
+        <v>925019</v>
       </c>
       <c r="D2" s="2">
         <f>(B2/C2)*A2*100</f>
-        <v>35.389548922974697</v>
+        <v>35.479843765371307</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
@@ -5812,6 +6129,66 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF5F47-D2FE-7143-818C-1205758ECD6B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2">
+        <v>4076</v>
+      </c>
+      <c r="C2" s="27">
+        <v>925019</v>
+      </c>
+      <c r="D2">
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.51</v>
+      </c>
+      <c r="F2">
+        <f>(D2/E2)*(B2/C2)*100</f>
+        <v>1.3141428001192725</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B76971B-B785-D444-906E-B14BE718062E}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -6013,7 +6390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637A7681-1608-124E-8520-29226F63BDFF}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -6228,192 +6605,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BAEB1E-CF2C-6A4E-B6C2-6EA04F34FC3D}">
-  <dimension ref="A1:K28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="2" width="10.625" style="1"/>
-    <col min="3" max="3" width="8.875" style="1" customWidth="1"/>
-    <col min="4" max="9" width="10.625" style="1"/>
-    <col min="10" max="10" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="18">
-      <c r="C1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1467.21</v>
-      </c>
-      <c r="E4" s="1">
-        <f>(SQRT(2*PI())*C6*C4)</f>
-        <v>4175.7542079112691</v>
-      </c>
-      <c r="G4" s="1">
-        <f>E9/E4</f>
-        <v>0.53247653583503463</v>
-      </c>
-      <c r="H4" s="1">
-        <f>E14/E4</f>
-        <v>0.5671611174999649</v>
-      </c>
-      <c r="J4" s="7">
-        <v>1443030</v>
-      </c>
-      <c r="K4" s="7">
-        <v>11382700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18">
-      <c r="C5" s="9">
-        <v>711.02300000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18">
-      <c r="C6" s="9">
-        <v>1.13541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="18">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="6">
-        <v>780.23099999999999</v>
-      </c>
-      <c r="E9" s="1">
-        <f>(SQRT(2*PI())*C11*C9)</f>
-        <v>2223.4911351271617</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18">
-      <c r="C10" s="6">
-        <v>709.88199999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="18">
-      <c r="C11" s="6">
-        <v>1.1369</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="I12" s="1">
-        <f>(J4/K4)*(H21/G4)*100</f>
-        <v>15.579447179280329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6">
-        <v>840.09100000000001</v>
-      </c>
-      <c r="E14" s="1">
-        <f>(SQRT(2*PI())*C16*C14)</f>
-        <v>2368.3254229641361</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="18">
-      <c r="C15" s="6">
-        <v>709.85400000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="18">
-      <c r="C16" s="6">
-        <v>1.1246700000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18">
-      <c r="C19" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18">
-      <c r="A21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="6">
-        <v>4558.08</v>
-      </c>
-      <c r="E21" s="1">
-        <f>(SQRT(2*PI())*C23*C21)</f>
-        <v>15138.785427111903</v>
-      </c>
-      <c r="H21" s="1">
-        <f>E26/E21</f>
-        <v>0.65436859451512963</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18">
-      <c r="C22" s="6">
-        <v>1348.17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18">
-      <c r="C23" s="6">
-        <v>1.32501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18">
-      <c r="A26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6">
-        <v>2999.78</v>
-      </c>
-      <c r="E26" s="1">
-        <f>(SQRT(2*PI())*C28*C26)</f>
-        <v>9906.3457426053428</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="18">
-      <c r="C27" s="6">
-        <v>1348.16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18">
-      <c r="C28" s="6">
-        <v>1.31745</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ring numbers and group cell to Sorter.C
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE13E6F-F3A4-2148-91D0-11E6F9C5E047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACE57B-0095-B64E-AF61-5425C30AD6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
   <sheets>
     <sheet name="Tri runs" sheetId="9" r:id="rId1"/>
@@ -676,7 +676,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -794,6 +794,13 @@
       <color theme="1"/>
       <name val="Menlo Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -853,7 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -895,6 +902,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers 2" xfId="2" xr:uid="{16FDB774-F211-F14E-9453-8C6A1F24C04D}"/>
@@ -1880,16 +1888,100 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4305300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BBC0EF3-34DA-C4CC-1AA3-EF0D2C0EB30D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6388100" y="1016000"/>
+          <a:ext cx="4953000" cy="660400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Avec la</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> méthode de Dmitry/Mathematica je trouve 37.7%</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1905,7 +1997,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7150100" y="368300"/>
-          <a:ext cx="2641600" cy="1397000"/>
+          <a:ext cx="4572000" cy="965200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1948,10 +2040,223 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1168400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="ZoneTexte 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE43851-F7E3-484B-87FA-6F66B50D80AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1168400" y="2882900"/>
+          <a:ext cx="5791200" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Avec méthode beta-n de BELEN</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> je trouve </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>P1n = 66.9% et P2n = 1.22%</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1400" baseline="0">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>P1n est aberrant mais P2n est correct.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Cette méthode doit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> être corrigé par l'efficacité du detecteur beta qui ne peut pas être moyennée.</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="ZoneTexte 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD032B7E-B84D-4641-8524-A232729C91AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="1244600"/>
+          <a:ext cx="4572000" cy="965200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Le</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> fit pour obtenir N2n est une somme d'exponentielle et pol0, à voir si c'est correct.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3281,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6376C050-E39F-4E43-B6D2-85F3F9FA265F}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4479,8 +4784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFFCE4E-1904-9441-B800-76A5932E8BAB}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5725,10 +6030,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EC6309-A58B-6542-A774-57FD4F318D67}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A16" sqref="A16:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5781,8 +6086,8 @@
         <v>0.57799999999999996</v>
       </c>
       <c r="C5" s="30">
-        <f>(A5/B5)*(B2/A2)</f>
-        <v>0.22505780958288429</v>
+        <f>(A5/B5)*(B2/A2)*100</f>
+        <v>22.50578095828843</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5815,6 +6120,25 @@
       <c r="D11" t="s">
         <v>196</v>
       </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="41"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="29"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="30"/>
+      <c r="C22" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6002,7 +6326,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6125,6 +6449,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6132,8 +6457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF5F47-D2FE-7143-818C-1205758ECD6B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6166,7 +6491,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2">
-        <v>4076</v>
+        <v>4158</v>
       </c>
       <c r="C2" s="27">
         <v>925019</v>
@@ -6175,11 +6500,11 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="E2">
-        <v>0.51</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="F2">
         <f>(D2/E2)*(B2/C2)*100</f>
-        <v>1.3141428001192725</v>
+        <v>1.3353437706414677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding analysis of 125Ag
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACE57B-0095-B64E-AF61-5425C30AD6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968567F0-F835-634B-9479-7C8E682B4D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
   <sheets>
     <sheet name="Tri runs" sheetId="9" r:id="rId1"/>
@@ -2178,14 +2178,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2201,7 +2201,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905500" y="1244600"/>
+          <a:off x="6819900" y="1701800"/>
           <a:ext cx="4572000" cy="965200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3586,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6376C050-E39F-4E43-B6D2-85F3F9FA265F}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4784,7 +4784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFFCE4E-1904-9441-B800-76A5932E8BAB}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -6150,7 +6150,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6326,7 +6326,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6365,14 +6365,14 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="B2" s="27">
-        <v>215776</v>
+        <v>223874</v>
       </c>
       <c r="C2" s="27">
-        <v>925019</v>
+        <v>961595</v>
       </c>
       <c r="D2" s="2">
         <f>(B2/C2)*A2*100</f>
-        <v>35.479843765371307</v>
+        <v>35.411202637284923</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
@@ -6458,7 +6458,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6491,10 +6491,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2">
-        <v>4158</v>
+        <v>17345</v>
       </c>
       <c r="C2" s="27">
-        <v>925019</v>
+        <v>961595</v>
       </c>
       <c r="D2">
         <v>1.5209999999999999</v>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="F2">
         <f>(D2/E2)*(B2/C2)*100</f>
-        <v>1.3353437706414677</v>
+        <v>5.3584768746847669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aligning One neutrons hists also, and pursuing analysis
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C07E21-9292-0D46-AAD3-65B24A12AFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A53DB-BDFF-7745-A958-97BAF9A4A245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
   <sheets>
     <sheet name="Tri runs" sheetId="9" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="209">
   <si>
     <t>Pn</t>
   </si>
@@ -668,6 +668,15 @@
   </si>
   <si>
     <t>64,65,66,67,68,69</t>
+  </si>
+  <si>
+    <t>beta-gamma</t>
+  </si>
+  <si>
+    <t>gamma single</t>
+  </si>
+  <si>
+    <t>eff beta</t>
   </si>
 </sst>
 </file>
@@ -2074,6 +2083,90 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2336800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2743200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="ZoneTexte 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F34BF7D-7DB1-E561-0121-C3800DB419BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2336800" y="2552700"/>
+          <a:ext cx="7442200" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Ici dans mon fit beta je prend en compte la branche</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> 2n</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2087,10 +2180,10 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2106,7 +2199,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7150100" y="368300"/>
-          <a:ext cx="4572000" cy="965200"/>
+          <a:ext cx="6502400" cy="2844800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2144,6 +2237,65 @@
             </a:rPr>
             <a:t>Ici j'ai pris le ratio calculé pour Pn 84Ga et j'ai pris Effn qui conserve ce ratio avec l'efficacité beta de 82Ga</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Pour cette méthode je fit la courbe d'activité des évenements 2 neutrons et</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> je fais le calcul P2n=(N2n/Nb)*Ratio*(1/Effn)</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1400" baseline="0">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" baseline="0">
+              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>En prenant la méthode statistique, efficacité beta du 82Ga et efficacité tetra = 0.512, ce qui conserve le ratio, je trouve 2.2% ce qui semble correct.</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1400">
+            <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2279,84 +2431,6 @@
             <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
             <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="ZoneTexte 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD032B7E-B84D-4641-8524-A232729C91AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6819900" y="1701800"/>
-          <a:ext cx="4572000" cy="965200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1400">
-              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>Le</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1400" baseline="0">
-              <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t> fit pour obtenir N2n est une somme de deux exponentielles.</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4114,7 +4188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6376C050-E39F-4E43-B6D2-85F3F9FA265F}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -5312,7 +5386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFFCE4E-1904-9441-B800-76A5932E8BAB}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -6679,7 +6753,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6854,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A42E313-E47F-404F-9F81-3A86BAAE3BBF}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6894,14 +6968,14 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="B2" s="27">
-        <v>223874</v>
+        <v>223756</v>
       </c>
       <c r="C2" s="27">
         <v>975418</v>
       </c>
       <c r="D2" s="2">
         <f>(B2/C2)*A2*100</f>
-        <v>34.90937772319149</v>
+        <v>34.890977611649568</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
@@ -6986,8 +7060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF5F47-D2FE-7143-818C-1205758ECD6B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -7020,10 +7094,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2">
-        <v>17345</v>
+        <v>6162</v>
       </c>
       <c r="C2" s="27">
-        <v>961595</v>
+        <v>975418</v>
       </c>
       <c r="D2">
         <v>1.5209999999999999</v>
@@ -7033,7 +7107,7 @@
       </c>
       <c r="F2">
         <f>(D2/E2)*(B2/C2)*100</f>
-        <v>5.3584768746847669</v>
+        <v>1.8766798086820211</v>
       </c>
     </row>
   </sheetData>
@@ -7044,12 +7118,105 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2ED87E-3B64-C24F-AC59-0C835EBF5EDA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="27">
+        <v>771.99599999999998</v>
+      </c>
+      <c r="B3" s="29">
+        <v>888.31399999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="27">
+        <v>383.93599999999998</v>
+      </c>
+      <c r="B4" s="29">
+        <v>383.96199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="27">
+        <v>0.97599599999999997</v>
+      </c>
+      <c r="B5" s="29">
+        <v>0.92991699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <f>SQRT(2*PI())*A3*A5</f>
+        <v>1888.6566930379788</v>
+      </c>
+      <c r="B7">
+        <f>SQRT(2*PI())*B3*B5</f>
+        <v>2070.6210660519237</v>
+      </c>
+      <c r="D7">
+        <f>A7/B7</f>
+        <v>0.91212087233281247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="27">
+        <v>231.80199999999999</v>
+      </c>
+      <c r="B9" s="29">
+        <v>281.78399999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="27">
+        <v>643.24699999999996</v>
+      </c>
+      <c r="B10" s="29">
+        <v>643.19299999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="27">
+        <v>0.93245599999999995</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1.00098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <f>SQRT(2*PI())*A9*A11</f>
+        <v>541.79558379850221</v>
+      </c>
+      <c r="B13">
+        <f>SQRT(2*PI())*B9*B11</f>
+        <v>707.01994292552558</v>
+      </c>
+      <c r="D13">
+        <f>A13/B13</f>
+        <v>0.76630877137163389</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Organizing different analyzer files into folders and changing n-n code so that it goes to last neutron seen after while
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A53DB-BDFF-7745-A958-97BAF9A4A245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903AB227-8445-F843-849E-E6988ABDAFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
   <sheets>
     <sheet name="Tri runs" sheetId="9" r:id="rId1"/>
@@ -872,7 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -921,6 +921,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers 2" xfId="2" xr:uid="{16FDB774-F211-F14E-9453-8C6A1F24C04D}"/>
@@ -2086,15 +2087,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2336800</xdr:colOff>
+      <xdr:colOff>2108200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2743200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>3302000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2109,8 +2110,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2336800" y="2552700"/>
-          <a:ext cx="7442200" cy="2286000"/>
+          <a:off x="2108200" y="2540000"/>
+          <a:ext cx="8229600" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,7 +2148,7 @@
               <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>Ici dans mon fit beta je prend en compte la branche</a:t>
+            <a:t>Dans mon fit beta je prend en compte la branche</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1400" baseline="0">
@@ -2155,7 +2156,7 @@
               <a:ea typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
               <a:cs typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t> 2n</a:t>
+            <a:t> beta-2n aussi.</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1400">
             <a:latin typeface="Menlo" panose="020B0609030804020204" pitchFamily="49" charset="0"/>
@@ -2816,7 +2817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6887EF2-46CF-E446-B33F-5F6D80182EE1}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4188,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6376C050-E39F-4E43-B6D2-85F3F9FA265F}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5386,7 +5387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFFCE4E-1904-9441-B800-76A5932E8BAB}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -6635,7 +6636,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6726,12 +6727,18 @@
     <row r="16" spans="1:4">
       <c r="A16" s="40"/>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="27"/>
+    </row>
     <row r="18" spans="1:3">
       <c r="A18" s="31"/>
       <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="29"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="44"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="31"/>
@@ -6926,10 +6933,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A42E313-E47F-404F-9F81-3A86BAAE3BBF}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6968,14 +6975,14 @@
         <v>1.5209999999999999</v>
       </c>
       <c r="B2" s="27">
-        <v>223756</v>
+        <v>218252</v>
       </c>
       <c r="C2" s="27">
-        <v>975418</v>
+        <v>949000</v>
       </c>
       <c r="D2" s="2">
         <f>(B2/C2)*A2*100</f>
-        <v>34.890977611649568</v>
+        <v>34.980115068493149</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
@@ -7047,8 +7054,11 @@
       <c r="B12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="17" spans="4:4" ht="18">
+    <row r="17" spans="3:4" ht="18">
       <c r="D17" s="3"/>
+    </row>
+    <row r="24" spans="3:4" ht="18">
+      <c r="C24" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7060,8 +7070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF5F47-D2FE-7143-818C-1205758ECD6B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -7097,7 +7107,7 @@
         <v>6162</v>
       </c>
       <c r="C2" s="27">
-        <v>975418</v>
+        <v>949000</v>
       </c>
       <c r="D2">
         <v>1.5209999999999999</v>
@@ -7107,7 +7117,7 @@
       </c>
       <c r="F2">
         <f>(D2/E2)*(B2/C2)*100</f>
-        <v>1.8766798086820211</v>
+        <v>1.9289223030821916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plot of random rate for 82 and 84 Ga in /divers
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantacuzene/n-ri-22/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918B913A-997D-FA4A-AD0C-04C5CB0F57BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8932DCF4-D820-4D45-A961-5099685EBD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{E76A3D8A-04E9-2843-901E-00CE4EC30078}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Eff 82Ga" sheetId="5" r:id="rId3"/>
     <sheet name="Pn 82Ga" sheetId="16" r:id="rId4"/>
     <sheet name="Eff 84Ga" sheetId="15" r:id="rId5"/>
-    <sheet name="&lt;n&gt; 84Ga" sheetId="14" r:id="rId6"/>
+    <sheet name="&lt;n&gt;  84Ga" sheetId="14" r:id="rId6"/>
     <sheet name="P1n 84Ga" sheetId="20" r:id="rId7"/>
     <sheet name="P2n 84Ga" sheetId="17" r:id="rId8"/>
     <sheet name="Eff 125Ag" sheetId="18" r:id="rId9"/>
@@ -6146,7 +6146,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6329,7 +6329,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6361,21 +6361,16 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2">
-        <v>30033</v>
-      </c>
-      <c r="C2" s="22">
-        <v>1107360</v>
-      </c>
+      <c r="C2" s="22"/>
       <c r="D2">
         <v>1.611</v>
       </c>
       <c r="E2">
         <v>0.45390000000000003</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="e">
         <f>(D2/E2)*(B2/C2)*100</f>
-        <v>9.6259863583662</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:7">

</xml_diff>